<commit_message>
Graphing program ready to be used, Changed name fuselage_design to initialsizing_fuselage
</commit_message>
<xml_diff>
--- a/Graphing/example.xlsx
+++ b/Graphing/example.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\DSE\DSE-23\Graphing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="11_E48630AE7E3FB6F7A5580B17939DDD9C2AD99313" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8189351B-D613-4A59-83F3-DB55173B7936}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_E48630AE7E3FB6F7A5580B17939DDD9C2AD99313" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{356470FC-BD5B-40A2-B358-F5E6C2CFAAB7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5016" yWindow="960" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Labels</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Number of passengers vs MTOW</t>
-  </si>
-  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>plot/scatter</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Label 3</t>
+  </si>
+  <si>
+    <t>Title example</t>
   </si>
 </sst>
 </file>
@@ -163,10 +169,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -827,7 +833,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -845,10 +851,10 @@
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -869,10 +875,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -910,12 +916,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -941,7 +949,10 @@
         <f>C7*1.2-5000</f>
         <v>35822.799999999996</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <f>0.5*D7</f>
+        <v>17911.399999999998</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -961,10 +972,13 @@
         <v>38330</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D26" si="0">C8*1.2-5000</f>
+        <f t="shared" ref="D8:D25" si="0">C8*1.2-5000</f>
         <v>40996</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8:E25" si="1">0.5*D8</f>
+        <v>20498</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -987,7 +1001,10 @@
         <f t="shared" si="0"/>
         <v>44968</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>22484</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1010,7 +1027,10 @@
         <f t="shared" si="0"/>
         <v>35822.799999999996</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>17911.399999999998</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1033,6 +1053,10 @@
         <f t="shared" si="0"/>
         <v>21400</v>
       </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>10700</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1055,6 +1079,10 @@
         <f t="shared" si="0"/>
         <v>23920</v>
       </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>11960</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="I12" s="1"/>
@@ -1076,6 +1104,10 @@
         <f t="shared" si="0"/>
         <v>41320</v>
       </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>20660</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="J13" s="1"/>
@@ -1096,6 +1128,10 @@
         <f t="shared" si="0"/>
         <v>43444</v>
       </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>21722</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="J14" s="1"/>
@@ -1116,6 +1152,10 @@
         <f t="shared" si="0"/>
         <v>57160</v>
       </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>28580</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="J15" s="1"/>
@@ -1136,6 +1176,10 @@
         <f t="shared" si="0"/>
         <v>57748</v>
       </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>28874</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="J16" s="1"/>
@@ -1156,6 +1200,10 @@
         <f t="shared" si="0"/>
         <v>48760</v>
       </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>24380</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="J17" s="1"/>
@@ -1176,6 +1224,10 @@
         <f t="shared" si="0"/>
         <v>62680</v>
       </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>31340</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="J18" s="1"/>
@@ -1196,6 +1248,10 @@
         <f t="shared" si="0"/>
         <v>68800</v>
       </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>34400</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="J19" s="1"/>
@@ -1216,6 +1272,10 @@
         <f t="shared" si="0"/>
         <v>43240</v>
       </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>21620</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="J20" s="1"/>
@@ -1236,6 +1296,10 @@
         <f t="shared" si="0"/>
         <v>46360</v>
       </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>23180</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="J21" s="1"/>
@@ -1255,6 +1319,10 @@
       <c r="D22" s="1">
         <f t="shared" si="0"/>
         <v>67937.2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>33968.6</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1277,6 +1345,10 @@
         <f t="shared" si="0"/>
         <v>47200</v>
       </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>23600</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1298,6 +1370,10 @@
         <f t="shared" si="0"/>
         <v>51618.400000000001</v>
       </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>25809.200000000001</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1318,7 +1394,10 @@
         <f t="shared" si="0"/>
         <v>47440</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>23720</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1348,37 +1427,40 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="D27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>